<commit_message>
L02f,L02g and L03A data,mapping,link files updated
</commit_message>
<xml_diff>
--- a/input files/L02F/L02F-Link.xlsx
+++ b/input files/L02F/L02F-Link.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Thomascook\current\Landing Page App\tc-exp-landing-pages\htmlGenerator3\sample files\L02F\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\htmlGenerator3\input files\L02G\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -80,11 +80,10 @@
     <t>TN_Section</t>
   </si>
   <si>
-    <t>&lt;div class="col-md-4"&gt;
-  &lt;div&gt;&lt;img src="#TN_SRC" alt="#TN_ALT"&gt;&lt;/div&gt;
+    <t>&lt;div  class="col-md-3 col-sm-3 col-xs-4 mb-block"&gt;&lt;img src="#TN_SRC"  class="tn-image" alt="#TN_ALT"&gt;
  &lt;div&gt;&lt;label class="h3-36" &gt;#TN_NAME&lt;/label&gt;&lt;/div&gt;
- &lt;div id="div_TN_Description" class="seo-text"&gt;#TN_DESC&lt;/div&gt;
- &lt;div id="div_Text_under_TN"&gt;&lt;a href="#UNDER_URL"&gt;#UNDER_TEXT&lt;/a&gt;&lt;/div&gt;
+ &lt;div class="seo-text"&gt;#TN_DESC&lt;/div&gt;
+ &lt;div&gt;&lt;a href="#UNDER_URL"&gt;#UNDER_TEXT&lt;/a&gt;&lt;/div&gt;
 &lt;/div&gt;</t>
   </si>
 </sst>
@@ -474,7 +473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -515,7 +514,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>

</xml_diff>